<commit_message>
Added a 'bucket' column to opportunity score
This round of update includes the following changes
     - Germnay was removed from the list of unique countries as the
       organisation did its work in Guatemala
     - Included a bucket variable in the opportunity_score.csv file
       which is a alphabetical variables classifyng countries as High,
       Medium, Low and Lowest opportunity countries based on the
       final score.
     - The above two changes have been reflected in the code
</commit_message>
<xml_diff>
--- a/data/input/unique_registry_responses.xlsx
+++ b/data/input/unique_registry_responses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nishka_sharma/Desktop/AQLI/aq_data_gap/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EEF5D82-B0B4-D249-AB60-EE83BF0C40D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831FE84C-05B8-A347-BD2F-03F65950E5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8340" yWindow="500" windowWidth="20460" windowHeight="15960" xr2:uid="{16875F82-30FE-C049-A2A1-A93273877366}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Guatemala</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>Angola</t>
-  </si>
-  <si>
-    <t>Germany</t>
   </si>
   <si>
     <t>Gambia</t>
@@ -192,10 +189,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -511,215 +506,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2231D2-B904-E045-8586-DBCCFA4A2518}">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
+      <c r="A1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
+      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>